<commit_message>
Commit for first publish
</commit_message>
<xml_diff>
--- a/Documents/Utilities #1 look up list.xlsx
+++ b/Documents/Utilities #1 look up list.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mewinter\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jsavory\Documents\GitHub\EA-FCRM-Utilities\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="7875" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Kent and South London" sheetId="1" r:id="rId1"/>
+    <sheet name="KSL" sheetId="1" r:id="rId1"/>
     <sheet name="Next Region" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>BT</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Service</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Direct Search</t>
   </si>
 </sst>
 </file>
@@ -426,52 +435,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -482,73 +522,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -818,20 +878,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <cf401361b24e474cb011be6eb76c0e76 xmlns="662745e8-e224-48e8-a2e3-254862b8c2f5">
@@ -891,6 +937,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="d1117845-93f6-4da3-abaa-fcb4fa669c78" ContentTypeId="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC01" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C276BF5-A48E-441D-AA7C-3AFD8B3B4AF5}">
   <ds:schemaRefs>
@@ -912,22 +972,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12469529-771F-44F6-8275-C55D3FC5E517}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F98BD90-7C9B-46E9-982A-7571F6632993}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D599A5ED-5420-423B-8224-B94E44B105C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -935,4 +979,20 @@
     <ds:schemaRef ds:uri="662745e8-e224-48e8-a2e3-254862b8c2f5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F98BD90-7C9B-46E9-982A-7571F6632993}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12469529-771F-44F6-8275-C55D3FC5E517}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>